<commit_message>
insert account, change password, change profile
</commit_message>
<xml_diff>
--- a/pl/testcase.xlsx
+++ b/pl/testcase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Database\SaleWebsite\pl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CDDDF0-AB5E-42A6-9920-9621E3D20518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDD021D-F2AA-468A-AAE7-193600E89CEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{044B5BA4-174B-4D2A-BD26-B2077AA82DF1}"/>
+    <workbookView xWindow="4755" yWindow="4275" windowWidth="21600" windowHeight="11325" xr2:uid="{044B5BA4-174B-4D2A-BD26-B2077AA82DF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -322,11 +322,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -644,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22DB11B0-55CF-4825-A24F-01EEA4DFEBEE}">
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +744,7 @@
       <c r="L2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>48</v>
       </c>
       <c r="N2" s="1" t="s">

</xml_diff>